<commit_message>
Pierwsza wersja (drobne uaktualnienia)
Dodano odpowiedzi na prawie 20 pytań
</commit_message>
<xml_diff>
--- a/UKE_porownanie_pytan.xlsx
+++ b/UKE_porownanie_pytan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafal\PycharmProjects\skrypty\UKE-nowe-pytania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A67B973-2A77-4705-8A0A-78A7C265A430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FAF325-4524-4CCE-9550-E7B028E851EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9942" uniqueCount="3701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9944" uniqueCount="3701">
   <si>
     <r>
       <t xml:space="preserve">Siła elektromotoryczna ogniwa wynosi 1,5 V. </t>
@@ -47815,7 +47815,9 @@
       <c r="G619" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H619" s="1"/>
+      <c r="H619" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="I619" s="1"/>
     </row>
     <row r="620" spans="1:9" x14ac:dyDescent="0.25">
@@ -59898,7 +59900,9 @@
       <c r="F496" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G496" s="1"/>
+      <c r="G496" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="H496" s="1"/>
     </row>
     <row r="497" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Porównanie z oficjalną wersją nowych pytań
</commit_message>
<xml_diff>
--- a/UKE_porownanie_pytan.xlsx
+++ b/UKE_porownanie_pytan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafal\PycharmProjects\skrypty\UKE-nowe-pytania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D5C86C-539A-4132-B234-6B3277710E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0C5F5D-7FAA-4354-972D-DC203289C99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,12 +23,25 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">porownanie!$A$1:$K$664</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">stare!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10483" uniqueCount="3434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10484" uniqueCount="3434">
   <si>
     <r>
       <t xml:space="preserve">Siła elektromotoryczna ogniwa wynosi 1,5 V. </t>
@@ -32573,7 +32586,9 @@
       <c r="H129" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="I129" s="2"/>
+      <c r="I129" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="J129" s="2"/>
       <c r="K129" s="7" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Oficjalne nowe a stare pytania - różnice
</commit_message>
<xml_diff>
--- a/UKE_porownanie_pytan.xlsx
+++ b/UKE_porownanie_pytan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafal\PycharmProjects\skrypty\UKE-nowe-pytania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BF62AF-5B6E-400B-8AAB-41EB77322F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AEF7F2-C2BD-4785-A695-84D580856302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28786,10 +28786,10 @@
   <dimension ref="A1:K664"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Poprawiono odpowiedzi na d1-289 i d1-306
Poprawiono odpowiedzi na nowe pytania d1-289 i d1-306
</commit_message>
<xml_diff>
--- a/UKE_porownanie_pytan.xlsx
+++ b/UKE_porownanie_pytan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafal\PycharmProjects\skrypty\UKE-nowe-pytania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216B67E8-0394-42D8-A43C-3078B910C4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87C400E-72C7-4370-BC2F-69049B03B980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14576" uniqueCount="3495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14580" uniqueCount="3497">
   <si>
     <r>
       <t xml:space="preserve">Siła elektromotoryczna ogniwa wynosi 1,5 V. </t>
@@ -28392,6 +28392,15 @@
   </si>
   <si>
     <t>[mrkobel] Prawidłowa odpowiedź to 2W (A, zamiast C). Również kalkulatory online podają taką odpowiedź jako prawidłową (np. https://www.everythingrf.com/rf-calculators/dbm-to-watts)</t>
+  </si>
+  <si>
+    <t>[mrkobel] wg. chat gpt prawidłowa odpowiedź to B.
+Więcej informacji również tutaj:
+https://sklep.delta.poznan.pl/dbi-zysk-energetyczny-anteny-izotropowej_l1_aid836.html</t>
+  </si>
+  <si>
+    <t>[mrkobel] Za Wikipedią:
+https://en.wikipedia.org/wiki/Maximum_usable_frequency</t>
   </si>
 </sst>
 </file>
@@ -40870,7 +40879,7 @@
       </c>
       <c r="O303" s="9"/>
     </row>
-    <row r="304" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>303</v>
       </c>
@@ -40892,9 +40901,11 @@
         <v>384</v>
       </c>
       <c r="I304" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J304" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="J304" s="2" t="s">
+        <v>3495</v>
+      </c>
       <c r="K304" s="7" t="s">
         <v>21</v>
       </c>
@@ -41533,7 +41544,7 @@
       </c>
       <c r="O320" s="9"/>
     </row>
-    <row r="321" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>320</v>
       </c>
@@ -41555,9 +41566,11 @@
         <v>367</v>
       </c>
       <c r="I321" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J321" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="J321" s="2" t="s">
+        <v>3496</v>
+      </c>
       <c r="K321" s="7" t="s">
         <v>21</v>
       </c>
@@ -75228,7 +75241,7 @@
       <c r="I290" s="1"/>
       <c r="J290" s="1"/>
     </row>
-    <row r="291" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>3009</v>
       </c>
@@ -75245,9 +75258,11 @@
         <v>384</v>
       </c>
       <c r="F291" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G291" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="G291" s="1" t="s">
+        <v>3495</v>
+      </c>
       <c r="H291" s="1" t="s">
         <v>1659</v>
       </c>
@@ -75730,7 +75745,7 @@
         <v>2689</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>2992</v>
       </c>
@@ -75747,9 +75762,11 @@
         <v>367</v>
       </c>
       <c r="F308" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G308" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="G308" s="1" t="s">
+        <v>3496</v>
+      </c>
       <c r="H308" s="1" t="s">
         <v>1659</v>
       </c>

</xml_diff>